<commit_message>
Update Map Interactions (#109)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Camping.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Camping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA6EABE-6FC0-4567-99A5-F4026B90115D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A88022-433F-4458-ACEF-1141C0381238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" activeTab="2" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
@@ -4121,10 +4121,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>마야! 토미! 쿠키도!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>마야?!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4162,6 +4158,10 @@
   </si>
   <si>
     <t>Tendency-철저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마야! 토미! 쿠키!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>20</v>
@@ -4862,7 +4862,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="10">
         <v>1</v>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>19</v>
@@ -4896,7 +4896,7 @@
         <v>70</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
@@ -4909,7 +4909,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>20</v>
@@ -5171,8 +5171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6CFE2B-C0F2-43E0-856F-54ADC42AF2F1}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5460,7 +5460,7 @@
         <v>70</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -5510,7 +5510,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -5538,7 +5538,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -5650,7 +5650,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
@@ -5821,7 +5821,7 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5832,7 +5832,7 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5979,7 +5979,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -5999,7 +5999,7 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6010,7 +6010,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -6144,7 +6144,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>

</xml_diff>